<commit_message>
commit only for satisfation
</commit_message>
<xml_diff>
--- a/excel-workbook.xlsx
+++ b/excel-workbook.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TICK\Downloads\Bots\whatsapp_bot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TICK\Desktop\Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Number</t>
   </si>
@@ -47,157 +47,31 @@
     <t>Message-5</t>
   </si>
   <si>
-    <t>post1.jpeg</t>
-  </si>
-  <si>
-    <t>Message 1</t>
-  </si>
-  <si>
-    <t>Message 2</t>
-  </si>
-  <si>
-    <t>Message 3</t>
-  </si>
-  <si>
-    <t>Message 4</t>
-  </si>
-  <si>
-    <t>Message 5</t>
-  </si>
-  <si>
-    <t>Message 6</t>
-  </si>
-  <si>
-    <t>Message 7</t>
-  </si>
-  <si>
-    <t>Message 8</t>
-  </si>
-  <si>
-    <t>Message 9</t>
-  </si>
-  <si>
-    <t>Message 10</t>
-  </si>
-  <si>
-    <t>Message 11</t>
-  </si>
-  <si>
-    <t>Message 12</t>
-  </si>
-  <si>
-    <t>Message 13</t>
-  </si>
-  <si>
-    <t>Message 14</t>
-  </si>
-  <si>
-    <t>Message 15</t>
-  </si>
-  <si>
-    <t>Message 16</t>
-  </si>
-  <si>
-    <t>Message 17</t>
-  </si>
-  <si>
-    <t>Message 18</t>
-  </si>
-  <si>
-    <t>Message 19</t>
-  </si>
-  <si>
-    <t>Message 20</t>
-  </si>
-  <si>
-    <t>Message 21</t>
-  </si>
-  <si>
-    <t>Message 22</t>
-  </si>
-  <si>
-    <t>Message 23</t>
-  </si>
-  <si>
-    <t>Message 24</t>
-  </si>
-  <si>
-    <t>Message 25</t>
-  </si>
-  <si>
-    <t>Message 26</t>
-  </si>
-  <si>
-    <t>Message 27</t>
-  </si>
-  <si>
-    <t>Message 28</t>
-  </si>
-  <si>
-    <t>Message 29</t>
-  </si>
-  <si>
-    <t>Message 30</t>
-  </si>
-  <si>
-    <t>Message 31</t>
-  </si>
-  <si>
-    <t>Message 32</t>
-  </si>
-  <si>
-    <t>Message 33</t>
-  </si>
-  <si>
-    <t>Message 34</t>
-  </si>
-  <si>
-    <t>Message 35</t>
-  </si>
-  <si>
-    <t>Message 36</t>
-  </si>
-  <si>
-    <t>Message 37</t>
-  </si>
-  <si>
-    <t>Message 38</t>
-  </si>
-  <si>
-    <t>Message 39</t>
-  </si>
-  <si>
-    <t>Message 40</t>
-  </si>
-  <si>
-    <t>Message 41</t>
-  </si>
-  <si>
-    <t>Message 42</t>
-  </si>
-  <si>
-    <t>Message 43</t>
-  </si>
-  <si>
-    <t>Message 44</t>
-  </si>
-  <si>
-    <t>Message 45</t>
-  </si>
-  <si>
-    <t>Message 46</t>
-  </si>
-  <si>
-    <t>Message 47</t>
-  </si>
-  <si>
-    <t>Message 48</t>
-  </si>
-  <si>
-    <t>Message 49</t>
-  </si>
-  <si>
-    <t>Message 50</t>
+    <t>reactjs</t>
+  </si>
+  <si>
+    <t>C:\Users\TICK\Desktop\Bot\bot icon.pdf</t>
+  </si>
+  <si>
+    <t>I am bot</t>
+  </si>
+  <si>
+    <t>did you like my phography?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi Again </t>
+  </si>
+  <si>
+    <t>Again I am here</t>
+  </si>
+  <si>
+    <t>Check this pdf</t>
+  </si>
+  <si>
+    <t>C:\Users\TICK\Desktop\Bot\clouds.jpg</t>
+  </si>
+  <si>
+    <t>Hello Sameer</t>
   </si>
 </sst>
 </file>
@@ -605,13 +479,14 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28" style="1" customWidth="1"/>
     <col min="7" max="7" width="71.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -643,22 +518,18 @@
         <v>3302085537</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>18</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>38</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -666,207 +537,93 @@
         <v>3302085537</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3302085537</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>3302085537</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>3302085537</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>3302085537</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>3302085537</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>3302085537</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>3302085537</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>3302085537</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>